<commit_message>
Correccion Perfil de proyecto
</commit_message>
<xml_diff>
--- a/1. Documentos/Itinerario.xlsx
+++ b/1. Documentos/Itinerario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nando\Documents\Carpeta de Nando\PRACTICAS PRE PROFESIONALES\Carpeta Tutora Practicas\Practicas Pre Profesionales\1. Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E834184-6C8E-4AE4-8104-C84EEE91FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3303104-6C45-46A4-8378-B35D3F53E8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="135">
   <si>
     <t>FECHA</t>
   </si>
@@ -715,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -748,161 +748,148 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1186,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1202,14 +1189,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24.6" x14ac:dyDescent="0.6">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
@@ -1245,2258 +1232,2250 @@
     </row>
     <row r="7" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="8" spans="1:7" ht="52.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="21" t="s">
+      <c r="E8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="36">
+      <c r="A9" s="51">
         <v>45761</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="14">
-        <v>2</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="27">
+      <c r="D9" s="13">
+        <v>2</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="49">
         <v>6</v>
       </c>
-      <c r="G9" s="30">
+      <c r="G9" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A10" s="37"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="15" t="s">
+      <c r="A10" s="46"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="15">
-        <v>2</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="30">
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="43"/>
+      <c r="G10" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="38"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="22" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="22">
-        <v>2</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="31">
+      <c r="D11" s="18">
+        <v>2</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="44"/>
+      <c r="G11" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="54.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="47">
+      <c r="A12" s="45">
         <v>45762</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="39">
-        <v>2</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="27">
+      <c r="D12" s="24">
+        <v>2</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="49">
         <v>6</v>
       </c>
-      <c r="G12" s="45">
+      <c r="G12" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="36" x14ac:dyDescent="0.5">
-      <c r="A13" s="37"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="15" t="s">
+      <c r="A13" s="46"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="15">
-        <v>2</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="46">
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="43"/>
+      <c r="G13" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="38"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="22" t="s">
+      <c r="A14" s="47"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="22">
-        <v>2</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="31">
+      <c r="D14" s="18">
+        <v>2</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="44"/>
+      <c r="G14" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="36.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="47">
+      <c r="A15" s="45">
         <v>45763</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="29">
         <v>6.25E-2</v>
       </c>
-      <c r="E15" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="49">
+      <c r="E15" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="42">
         <v>6</v>
       </c>
-      <c r="G15" s="45">
+      <c r="G15" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A16" s="37"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="16" t="s">
+      <c r="A16" s="46"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="30">
         <v>6.25E-2</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="46">
+      <c r="E16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="43"/>
+      <c r="G16" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A17" s="37"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="16" t="s">
+      <c r="A17" s="46"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="15">
-        <v>2</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="46">
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="43"/>
+      <c r="G17" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="38"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="23" t="s">
+      <c r="A18" s="47"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="22">
-        <v>1</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="31">
+      <c r="D18" s="18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="44"/>
+      <c r="G18" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="36.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="47">
+      <c r="A19" s="45">
         <v>45768</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="24">
         <v>3</v>
       </c>
-      <c r="E19" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="49">
+      <c r="E19" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="42">
         <v>6</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G19" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="38"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="23" t="s">
+      <c r="A20" s="47"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="18">
         <v>3</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="29"/>
-      <c r="G20" s="31">
+      <c r="E20" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="44"/>
+      <c r="G20" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="36.6" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="47">
+      <c r="A21" s="45">
         <v>45769</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="24">
         <v>3</v>
       </c>
-      <c r="E21" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="49">
+      <c r="E21" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="42">
         <v>6</v>
       </c>
-      <c r="G21" s="45">
+      <c r="G21" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="38"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="22" t="s">
+      <c r="A22" s="47"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="18">
         <v>3</v>
       </c>
-      <c r="E22" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="31">
+      <c r="E22" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="44"/>
+      <c r="G22" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="54.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="47">
+      <c r="A23" s="45">
         <v>45770</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="39">
-        <v>2</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="49">
+      <c r="D23" s="24">
+        <v>2</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="42">
         <v>6</v>
       </c>
-      <c r="G23" s="45">
+      <c r="G23" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A24" s="37"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="15" t="s">
+      <c r="A24" s="46"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="15">
-        <v>2</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="46">
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="43"/>
+      <c r="G24" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A25" s="37"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="15" t="s">
+      <c r="A25" s="46"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="15">
-        <v>2</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="46">
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="43"/>
+      <c r="G25" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="38"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="22" t="s">
+      <c r="A26" s="47"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="22">
-        <v>2</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="31">
+      <c r="D26" s="18">
+        <v>2</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="44"/>
+      <c r="G26" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="36.6" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="47">
+      <c r="A27" s="45">
         <v>45771</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="39">
+      <c r="D27" s="24">
         <v>3</v>
       </c>
-      <c r="E27" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="49">
+      <c r="E27" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="42">
         <v>6</v>
       </c>
-      <c r="G27" s="45">
+      <c r="G27" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="38"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="22" t="s">
+      <c r="A28" s="47"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="18">
         <v>3</v>
       </c>
-      <c r="E28" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="29"/>
-      <c r="G28" s="31">
+      <c r="E28" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="44"/>
+      <c r="G28" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="36.6" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="47">
+      <c r="A29" s="45">
         <v>45772</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="39">
+      <c r="D29" s="24">
         <v>3</v>
       </c>
-      <c r="E29" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="49">
+      <c r="E29" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="42">
         <v>6</v>
       </c>
-      <c r="G29" s="45">
+      <c r="G29" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="38"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="22" t="s">
+      <c r="A30" s="47"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="18">
         <v>3</v>
       </c>
-      <c r="E30" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="31">
+      <c r="E30" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="44"/>
+      <c r="G30" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="57">
+      <c r="A31" s="31">
         <v>45775</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="59" t="s">
+      <c r="C31" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="59">
+      <c r="D31" s="33">
         <v>6</v>
       </c>
-      <c r="E31" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="60"/>
-      <c r="G31" s="61">
+      <c r="E31" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="34"/>
+      <c r="G31" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="47">
+      <c r="A32" s="45">
         <v>45776</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="39">
-        <v>2</v>
-      </c>
-      <c r="E32" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="49">
+      <c r="D32" s="24">
+        <v>2</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="42">
         <v>6</v>
       </c>
-      <c r="G32" s="45">
+      <c r="G32" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A33" s="37"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="15" t="s">
+      <c r="A33" s="46"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="15">
-        <v>2</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="28"/>
-      <c r="G33" s="46">
+      <c r="D33" s="4">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="43"/>
+      <c r="G33" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="38"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="22" t="s">
+      <c r="A34" s="47"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="22">
-        <v>2</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="31">
+      <c r="D34" s="18">
+        <v>2</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="44"/>
+      <c r="G34" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="47">
+      <c r="A35" s="45">
         <v>45777</v>
       </c>
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C35" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="39">
+      <c r="D35" s="24">
         <v>3</v>
       </c>
-      <c r="E35" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="49">
+      <c r="E35" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="42">
         <v>6</v>
       </c>
-      <c r="G35" s="45">
+      <c r="G35" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="38"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="22" t="s">
+      <c r="A36" s="47"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="18">
         <v>3</v>
       </c>
-      <c r="E36" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="29"/>
-      <c r="G36" s="31">
+      <c r="E36" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="44"/>
+      <c r="G36" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="57">
+      <c r="A37" s="31">
         <v>45778</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="59" t="s">
+      <c r="C37" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="59">
+      <c r="D37" s="33">
         <v>6</v>
       </c>
-      <c r="E37" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="62">
+      <c r="E37" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="36">
         <v>6</v>
       </c>
-      <c r="G37" s="61">
+      <c r="G37" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="47">
+      <c r="A38" s="45">
         <v>45782</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="24">
         <v>3</v>
       </c>
-      <c r="E38" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="49">
+      <c r="E38" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="42">
         <v>6</v>
       </c>
-      <c r="G38" s="45">
+      <c r="G38" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="38"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="22" t="s">
+      <c r="A39" s="47"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="18">
         <v>3</v>
       </c>
-      <c r="E39" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" s="29"/>
-      <c r="G39" s="31">
+      <c r="E39" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="44"/>
+      <c r="G39" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="47">
+      <c r="A40" s="45">
         <v>45783</v>
       </c>
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="C40" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="39">
+      <c r="D40" s="24">
         <v>3</v>
       </c>
-      <c r="E40" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="49">
+      <c r="E40" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="42">
         <v>6</v>
       </c>
-      <c r="G40" s="45">
+      <c r="G40" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="38"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="22" t="s">
+      <c r="A41" s="47"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="18">
         <v>3</v>
       </c>
-      <c r="E41" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="29"/>
-      <c r="G41" s="31">
+      <c r="E41" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="44"/>
+      <c r="G41" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="57">
+      <c r="A42" s="31">
         <v>45784</v>
       </c>
-      <c r="B42" s="58" t="s">
+      <c r="B42" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="59" t="s">
+      <c r="C42" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D42" s="59">
+      <c r="D42" s="33">
         <v>6</v>
       </c>
-      <c r="E42" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" s="62">
+      <c r="E42" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="36">
         <v>6</v>
       </c>
-      <c r="G42" s="61">
+      <c r="G42" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="47">
+      <c r="A43" s="45">
         <v>45785</v>
       </c>
-      <c r="B43" s="48" t="s">
+      <c r="B43" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="39">
-        <v>2</v>
-      </c>
-      <c r="E43" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F43" s="49">
+      <c r="D43" s="24">
+        <v>2</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="42">
         <v>4</v>
       </c>
-      <c r="G43" s="45">
+      <c r="G43" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="38"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="22" t="s">
+      <c r="A44" s="47"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D44" s="22">
-        <v>2</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F44" s="29"/>
-      <c r="G44" s="31">
+      <c r="D44" s="18">
+        <v>2</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="44"/>
+      <c r="G44" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="57">
+      <c r="A45" s="31">
         <v>45789</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="D45" s="59">
+      <c r="D45" s="33">
         <v>4</v>
       </c>
-      <c r="E45" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" s="62">
+      <c r="E45" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="36">
         <v>4</v>
       </c>
-      <c r="G45" s="61">
+      <c r="G45" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="47">
+      <c r="A46" s="45">
         <v>45790</v>
       </c>
-      <c r="B46" s="48" t="s">
+      <c r="B46" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="C46" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="39">
-        <v>1</v>
-      </c>
-      <c r="E46" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F46" s="49">
+      <c r="D46" s="24">
+        <v>1</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="42">
         <v>4</v>
       </c>
-      <c r="G46" s="45">
+      <c r="G46" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A47" s="37"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="15" t="s">
+      <c r="A47" s="46"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D47" s="55">
+      <c r="D47" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E47" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F47" s="28"/>
-      <c r="G47" s="46">
+      <c r="E47" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="43"/>
+      <c r="G47" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A48" s="37"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="15" t="s">
+      <c r="A48" s="46"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="55">
+      <c r="D48" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="46">
+      <c r="E48" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="43"/>
+      <c r="G48" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A49" s="37"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="15" t="s">
+      <c r="A49" s="46"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D49" s="15">
-        <v>1</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F49" s="28"/>
-      <c r="G49" s="46">
+      <c r="D49" s="4">
+        <v>1</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="43"/>
+      <c r="G49" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="38"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="22" t="s">
+      <c r="A50" s="47"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D50" s="22">
-        <v>1</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="29"/>
-      <c r="G50" s="31">
+      <c r="D50" s="18">
+        <v>1</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="44"/>
+      <c r="G50" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="47">
+      <c r="A51" s="45">
         <v>45791</v>
       </c>
-      <c r="B51" s="48" t="s">
+      <c r="B51" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="39" t="s">
+      <c r="C51" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="54">
+      <c r="D51" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E51" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" s="49">
+      <c r="E51" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="42">
         <v>4</v>
       </c>
-      <c r="G51" s="45">
+      <c r="G51" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A52" s="37"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="15" t="s">
+      <c r="A52" s="46"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D52" s="55">
+      <c r="D52" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E52" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="28"/>
-      <c r="G52" s="46">
+      <c r="E52" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" s="43"/>
+      <c r="G52" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A53" s="37"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="15" t="s">
+      <c r="A53" s="46"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="55">
+      <c r="D53" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E53" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F53" s="28"/>
-      <c r="G53" s="46">
+      <c r="E53" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="43"/>
+      <c r="G53" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A54" s="37"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="15" t="s">
+      <c r="A54" s="46"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D54" s="55">
+      <c r="D54" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E54" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F54" s="28"/>
-      <c r="G54" s="46">
+      <c r="E54" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="43"/>
+      <c r="G54" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A55" s="37"/>
-      <c r="B55" s="34"/>
-      <c r="C55" s="15" t="s">
+      <c r="A55" s="46"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="55">
+      <c r="D55" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E55" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F55" s="28"/>
-      <c r="G55" s="46">
+      <c r="E55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="43"/>
+      <c r="G55" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A56" s="37"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="15" t="s">
+      <c r="A56" s="46"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D56" s="55">
+      <c r="D56" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E56" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F56" s="28"/>
-      <c r="G56" s="46">
+      <c r="E56" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="43"/>
+      <c r="G56" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A57" s="37"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="15" t="s">
+      <c r="A57" s="46"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D57" s="55">
+      <c r="D57" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E57" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F57" s="28"/>
-      <c r="G57" s="46">
+      <c r="E57" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="43"/>
+      <c r="G57" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="38"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="22" t="s">
+      <c r="A58" s="47"/>
+      <c r="B58" s="41"/>
+      <c r="C58" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D58" s="63">
+      <c r="D58" s="37">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E58" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F58" s="29"/>
-      <c r="G58" s="31">
+      <c r="E58" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F58" s="44"/>
+      <c r="G58" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="37">
+      <c r="A59" s="46">
         <v>45792</v>
       </c>
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D59" s="15">
-        <v>1</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" s="28">
+      <c r="D59" s="4">
+        <v>1</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" s="43">
         <v>4</v>
       </c>
-      <c r="G59" s="46">
+      <c r="G59" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A60" s="37"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="15" t="s">
+      <c r="A60" s="46"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D60" s="15">
-        <v>1</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="28"/>
-      <c r="G60" s="46">
+      <c r="D60" s="4">
+        <v>1</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" s="43"/>
+      <c r="G60" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A61" s="37"/>
-      <c r="B61" s="34"/>
-      <c r="C61" s="15" t="s">
+      <c r="A61" s="46"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="15">
-        <v>1</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F61" s="28"/>
-      <c r="G61" s="46">
+      <c r="D61" s="4">
+        <v>1</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="43"/>
+      <c r="G61" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="38"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="22" t="s">
+      <c r="A62" s="47"/>
+      <c r="B62" s="41"/>
+      <c r="C62" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D62" s="22">
-        <v>1</v>
-      </c>
-      <c r="E62" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F62" s="29"/>
-      <c r="G62" s="31">
+      <c r="D62" s="18">
+        <v>1</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" s="44"/>
+      <c r="G62" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="47">
+      <c r="A63" s="45">
         <v>45793</v>
       </c>
-      <c r="B63" s="48" t="s">
+      <c r="B63" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C63" s="39" t="s">
+      <c r="C63" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D63" s="54">
+      <c r="D63" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E63" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F63" s="49">
+      <c r="E63" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" s="42">
         <v>4</v>
       </c>
-      <c r="G63" s="45">
+      <c r="G63" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A64" s="37"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="15" t="s">
+      <c r="A64" s="46"/>
+      <c r="B64" s="40"/>
+      <c r="C64" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D64" s="55">
+      <c r="D64" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E64" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="28"/>
-      <c r="G64" s="46">
+      <c r="E64" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="43"/>
+      <c r="G64" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A65" s="37"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="15" t="s">
+      <c r="A65" s="46"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D65" s="55">
+      <c r="D65" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E65" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F65" s="28"/>
-      <c r="G65" s="46">
+      <c r="E65" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="43"/>
+      <c r="G65" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A66" s="37"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="15" t="s">
+      <c r="A66" s="46"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D66" s="55">
+      <c r="D66" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E66" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F66" s="28"/>
-      <c r="G66" s="46">
+      <c r="E66" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" s="43"/>
+      <c r="G66" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A67" s="37"/>
-      <c r="B67" s="34"/>
-      <c r="C67" s="15" t="s">
+      <c r="A67" s="46"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D67" s="55">
+      <c r="D67" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E67" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F67" s="28"/>
-      <c r="G67" s="46">
+      <c r="E67" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" s="43"/>
+      <c r="G67" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A68" s="37"/>
-      <c r="B68" s="34"/>
-      <c r="C68" s="15" t="s">
+      <c r="A68" s="46"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D68" s="55">
+      <c r="D68" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E68" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F68" s="28"/>
-      <c r="G68" s="46">
+      <c r="E68" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" s="43"/>
+      <c r="G68" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A69" s="37"/>
-      <c r="B69" s="34"/>
-      <c r="C69" s="15" t="s">
+      <c r="A69" s="46"/>
+      <c r="B69" s="40"/>
+      <c r="C69" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D69" s="55">
+      <c r="D69" s="30">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E69" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F69" s="28"/>
-      <c r="G69" s="46">
+      <c r="E69" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F69" s="43"/>
+      <c r="G69" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="38"/>
-      <c r="B70" s="35"/>
-      <c r="C70" s="22" t="s">
+      <c r="A70" s="47"/>
+      <c r="B70" s="41"/>
+      <c r="C70" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D70" s="63">
+      <c r="D70" s="37">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E70" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F70" s="29"/>
-      <c r="G70" s="31">
+      <c r="E70" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="44"/>
+      <c r="G70" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A71" s="47">
+      <c r="A71" s="45">
         <v>45796</v>
       </c>
-      <c r="B71" s="48" t="s">
+      <c r="B71" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="39" t="s">
+      <c r="C71" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="D71" s="39">
-        <v>1</v>
-      </c>
-      <c r="E71" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F71" s="49">
+      <c r="D71" s="24">
+        <v>1</v>
+      </c>
+      <c r="E71" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" s="42">
         <v>4</v>
       </c>
-      <c r="G71" s="45">
+      <c r="G71" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A72" s="37"/>
-      <c r="B72" s="34"/>
-      <c r="C72" s="15" t="s">
+      <c r="A72" s="46"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D72" s="15">
-        <v>2</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F72" s="28"/>
-      <c r="G72" s="46">
+      <c r="D72" s="4">
+        <v>2</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="43"/>
+      <c r="G72" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="38"/>
-      <c r="B73" s="35"/>
-      <c r="C73" s="22" t="s">
+      <c r="A73" s="47"/>
+      <c r="B73" s="41"/>
+      <c r="C73" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D73" s="22">
-        <v>1</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F73" s="29"/>
-      <c r="G73" s="31">
+      <c r="D73" s="18">
+        <v>1</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F73" s="44"/>
+      <c r="G73" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A74" s="47">
+      <c r="A74" s="45">
         <v>45797</v>
       </c>
-      <c r="B74" s="48" t="s">
+      <c r="B74" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="C74" s="39" t="s">
+      <c r="C74" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D74" s="39">
-        <v>1</v>
-      </c>
-      <c r="E74" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F74" s="49">
+      <c r="D74" s="24">
+        <v>1</v>
+      </c>
+      <c r="E74" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="42">
         <v>4</v>
       </c>
-      <c r="G74" s="45">
+      <c r="G74" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A75" s="37"/>
-      <c r="B75" s="34"/>
-      <c r="C75" s="15" t="s">
+      <c r="A75" s="46"/>
+      <c r="B75" s="40"/>
+      <c r="C75" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D75" s="15">
-        <v>1</v>
-      </c>
-      <c r="E75" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F75" s="28"/>
-      <c r="G75" s="46">
+      <c r="D75" s="4">
+        <v>1</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" s="43"/>
+      <c r="G75" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="38"/>
-      <c r="B76" s="35"/>
-      <c r="C76" s="22" t="s">
+      <c r="A76" s="47"/>
+      <c r="B76" s="41"/>
+      <c r="C76" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D76" s="22">
-        <v>2</v>
-      </c>
-      <c r="E76" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F76" s="29"/>
-      <c r="G76" s="31">
+      <c r="D76" s="18">
+        <v>2</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F76" s="44"/>
+      <c r="G76" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A77" s="47">
+      <c r="A77" s="45">
         <v>45798</v>
       </c>
-      <c r="B77" s="48" t="s">
+      <c r="B77" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="C77" s="39" t="s">
+      <c r="C77" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D77" s="39">
-        <v>2</v>
-      </c>
-      <c r="E77" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F77" s="49">
+      <c r="D77" s="24">
+        <v>2</v>
+      </c>
+      <c r="E77" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" s="42">
         <v>4</v>
       </c>
-      <c r="G77" s="45">
+      <c r="G77" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A78" s="37"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="15" t="s">
+      <c r="A78" s="46"/>
+      <c r="B78" s="40"/>
+      <c r="C78" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D78" s="15">
-        <v>1</v>
-      </c>
-      <c r="E78" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F78" s="28"/>
-      <c r="G78" s="46">
+      <c r="D78" s="4">
+        <v>1</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78" s="43"/>
+      <c r="G78" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="38"/>
-      <c r="B79" s="35"/>
-      <c r="C79" s="22" t="s">
+      <c r="A79" s="47"/>
+      <c r="B79" s="41"/>
+      <c r="C79" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D79" s="22">
-        <v>1</v>
-      </c>
-      <c r="E79" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F79" s="29"/>
-      <c r="G79" s="31">
+      <c r="D79" s="18">
+        <v>1</v>
+      </c>
+      <c r="E79" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="44"/>
+      <c r="G79" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A80" s="47">
+      <c r="A80" s="45">
         <v>45803</v>
       </c>
-      <c r="B80" s="48" t="s">
+      <c r="B80" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="39" t="s">
+      <c r="C80" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="D80" s="39">
-        <v>2</v>
-      </c>
-      <c r="E80" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F80" s="49">
+      <c r="D80" s="24">
+        <v>2</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F80" s="42">
         <v>4</v>
       </c>
-      <c r="G80" s="45">
+      <c r="G80" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="38"/>
-      <c r="B81" s="35"/>
-      <c r="C81" s="22" t="s">
+      <c r="A81" s="47"/>
+      <c r="B81" s="41"/>
+      <c r="C81" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D81" s="22">
-        <v>2</v>
-      </c>
-      <c r="E81" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F81" s="29"/>
-      <c r="G81" s="31">
+      <c r="D81" s="18">
+        <v>2</v>
+      </c>
+      <c r="E81" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F81" s="44"/>
+      <c r="G81" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="57">
+      <c r="A82" s="31">
         <v>45804</v>
       </c>
-      <c r="B82" s="58" t="s">
+      <c r="B82" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C82" s="59" t="s">
+      <c r="C82" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="D82" s="59">
+      <c r="D82" s="33">
         <v>4</v>
       </c>
-      <c r="E82" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="F82" s="62">
+      <c r="E82" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F82" s="36">
         <v>4</v>
       </c>
-      <c r="G82" s="61">
+      <c r="G82" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A83" s="47">
+      <c r="A83" s="45">
         <v>45805</v>
       </c>
-      <c r="B83" s="48" t="s">
+      <c r="B83" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C83" s="39" t="s">
+      <c r="C83" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="D83" s="39">
-        <v>2</v>
-      </c>
-      <c r="E83" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F83" s="49">
+      <c r="D83" s="24">
+        <v>2</v>
+      </c>
+      <c r="E83" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F83" s="42">
         <v>4</v>
       </c>
-      <c r="G83" s="45">
+      <c r="G83" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A84" s="37"/>
-      <c r="B84" s="34"/>
-      <c r="C84" s="15" t="s">
+      <c r="A84" s="46"/>
+      <c r="B84" s="40"/>
+      <c r="C84" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D84" s="15">
-        <v>1</v>
-      </c>
-      <c r="E84" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F84" s="28"/>
-      <c r="G84" s="46">
+      <c r="D84" s="4">
+        <v>1</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F84" s="43"/>
+      <c r="G84" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="38"/>
-      <c r="B85" s="35"/>
-      <c r="C85" s="22" t="s">
+      <c r="A85" s="47"/>
+      <c r="B85" s="41"/>
+      <c r="C85" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D85" s="22">
-        <v>1</v>
-      </c>
-      <c r="E85" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F85" s="29"/>
-      <c r="G85" s="31">
+      <c r="D85" s="18">
+        <v>1</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85" s="44"/>
+      <c r="G85" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A86" s="47">
+      <c r="A86" s="45">
         <v>45779</v>
       </c>
-      <c r="B86" s="48" t="s">
+      <c r="B86" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C86" s="39" t="s">
+      <c r="C86" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D86" s="39">
-        <v>1</v>
-      </c>
-      <c r="E86" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F86" s="49">
+      <c r="D86" s="24">
+        <v>1</v>
+      </c>
+      <c r="E86" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F86" s="42">
         <v>4</v>
       </c>
-      <c r="G86" s="45">
+      <c r="G86" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A87" s="37"/>
-      <c r="B87" s="34"/>
-      <c r="C87" s="15" t="s">
+      <c r="A87" s="46"/>
+      <c r="B87" s="40"/>
+      <c r="C87" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D87" s="15">
-        <v>1</v>
-      </c>
-      <c r="E87" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F87" s="28"/>
-      <c r="G87" s="46">
+      <c r="D87" s="4">
+        <v>1</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F87" s="43"/>
+      <c r="G87" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A88" s="37"/>
-      <c r="B88" s="34"/>
-      <c r="C88" s="15" t="s">
+      <c r="A88" s="46"/>
+      <c r="B88" s="40"/>
+      <c r="C88" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D88" s="15">
-        <v>1</v>
-      </c>
-      <c r="E88" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F88" s="28"/>
-      <c r="G88" s="46">
+      <c r="D88" s="4">
+        <v>1</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" s="43"/>
+      <c r="G88" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="38"/>
-      <c r="B89" s="35"/>
-      <c r="C89" s="22" t="s">
+      <c r="A89" s="47"/>
+      <c r="B89" s="41"/>
+      <c r="C89" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D89" s="22">
-        <v>1</v>
-      </c>
-      <c r="E89" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F89" s="29"/>
-      <c r="G89" s="31">
+      <c r="D89" s="18">
+        <v>1</v>
+      </c>
+      <c r="E89" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F89" s="44"/>
+      <c r="G89" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A90" s="47">
+      <c r="A90" s="45">
         <v>45780</v>
       </c>
-      <c r="B90" s="48" t="s">
+      <c r="B90" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C90" s="39" t="s">
+      <c r="C90" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="D90" s="39">
-        <v>2</v>
-      </c>
-      <c r="E90" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F90" s="49">
+      <c r="D90" s="24">
+        <v>2</v>
+      </c>
+      <c r="E90" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F90" s="42">
         <v>4</v>
       </c>
-      <c r="G90" s="45">
+      <c r="G90" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="38"/>
-      <c r="B91" s="35"/>
-      <c r="C91" s="22" t="s">
+      <c r="A91" s="47"/>
+      <c r="B91" s="41"/>
+      <c r="C91" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D91" s="22">
-        <v>2</v>
-      </c>
-      <c r="E91" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F91" s="29"/>
-      <c r="G91" s="31">
+      <c r="D91" s="18">
+        <v>2</v>
+      </c>
+      <c r="E91" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F91" s="44"/>
+      <c r="G91" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A92" s="47">
+      <c r="A92" s="45">
         <v>45781</v>
       </c>
-      <c r="B92" s="48" t="s">
+      <c r="B92" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C92" s="39" t="s">
+      <c r="C92" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="D92" s="39">
-        <v>2</v>
-      </c>
-      <c r="E92" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F92" s="44">
+      <c r="D92" s="24">
+        <v>2</v>
+      </c>
+      <c r="E92" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F92" s="57">
         <v>4</v>
       </c>
-      <c r="G92" s="45">
+      <c r="G92" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="38"/>
-      <c r="B93" s="35"/>
-      <c r="C93" s="22" t="s">
+      <c r="A93" s="47"/>
+      <c r="B93" s="41"/>
+      <c r="C93" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D93" s="22">
-        <v>2</v>
-      </c>
-      <c r="E93" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F93" s="26"/>
-      <c r="G93" s="31">
+      <c r="D93" s="18">
+        <v>2</v>
+      </c>
+      <c r="E93" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F93" s="58"/>
+      <c r="G93" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A94" s="47">
+      <c r="A94" s="45">
         <v>45782</v>
       </c>
-      <c r="B94" s="48" t="s">
+      <c r="B94" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C94" s="39" t="s">
+      <c r="C94" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D94" s="39">
-        <v>2</v>
-      </c>
-      <c r="E94" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F94" s="44">
+      <c r="D94" s="24">
+        <v>2</v>
+      </c>
+      <c r="E94" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F94" s="57">
         <v>4</v>
       </c>
-      <c r="G94" s="45">
+      <c r="G94" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A95" s="37"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="15" t="s">
+      <c r="A95" s="46"/>
+      <c r="B95" s="40"/>
+      <c r="C95" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D95" s="15">
-        <v>1</v>
-      </c>
-      <c r="E95" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F95" s="25"/>
-      <c r="G95" s="46">
+      <c r="D95" s="4">
+        <v>1</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F95" s="59"/>
+      <c r="G95" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="38"/>
-      <c r="B96" s="35"/>
-      <c r="C96" s="22" t="s">
+      <c r="A96" s="47"/>
+      <c r="B96" s="41"/>
+      <c r="C96" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D96" s="22">
-        <v>1</v>
-      </c>
-      <c r="E96" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F96" s="26"/>
-      <c r="G96" s="31">
+      <c r="D96" s="18">
+        <v>1</v>
+      </c>
+      <c r="E96" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F96" s="58"/>
+      <c r="G96" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A97" s="47">
+      <c r="A97" s="45">
         <v>45783</v>
       </c>
-      <c r="B97" s="48" t="s">
+      <c r="B97" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C97" s="39" t="s">
+      <c r="C97" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D97" s="39">
-        <v>2</v>
-      </c>
-      <c r="E97" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F97" s="49">
+      <c r="D97" s="24">
+        <v>2</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F97" s="42">
         <v>4</v>
       </c>
-      <c r="G97" s="45">
+      <c r="G97" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A98" s="37"/>
-      <c r="B98" s="34"/>
-      <c r="C98" s="15" t="s">
+      <c r="A98" s="46"/>
+      <c r="B98" s="40"/>
+      <c r="C98" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D98" s="15">
-        <v>1</v>
-      </c>
-      <c r="E98" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F98" s="28"/>
-      <c r="G98" s="46">
+      <c r="D98" s="4">
+        <v>1</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F98" s="43"/>
+      <c r="G98" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="38"/>
-      <c r="B99" s="35"/>
-      <c r="C99" s="22" t="s">
+      <c r="A99" s="47"/>
+      <c r="B99" s="41"/>
+      <c r="C99" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D99" s="22">
-        <v>1</v>
-      </c>
-      <c r="E99" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F99" s="29"/>
-      <c r="G99" s="31">
+      <c r="D99" s="18">
+        <v>1</v>
+      </c>
+      <c r="E99" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F99" s="44"/>
+      <c r="G99" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A100" s="47">
+      <c r="A100" s="45">
         <v>45817</v>
       </c>
-      <c r="B100" s="48" t="s">
+      <c r="B100" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C100" s="39" t="s">
+      <c r="C100" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D100" s="39">
-        <v>2</v>
-      </c>
-      <c r="E100" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F100" s="49">
+      <c r="D100" s="24">
+        <v>2</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F100" s="42">
         <v>4</v>
       </c>
-      <c r="G100" s="45">
+      <c r="G100" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="38"/>
-      <c r="B101" s="35"/>
-      <c r="C101" s="22" t="s">
+      <c r="A101" s="47"/>
+      <c r="B101" s="41"/>
+      <c r="C101" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D101" s="22">
-        <v>2</v>
-      </c>
-      <c r="E101" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F101" s="29"/>
-      <c r="G101" s="31">
+      <c r="D101" s="18">
+        <v>2</v>
+      </c>
+      <c r="E101" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F101" s="44"/>
+      <c r="G101" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="57">
+      <c r="A102" s="31">
         <v>45818</v>
       </c>
-      <c r="B102" s="58" t="s">
+      <c r="B102" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C102" s="59" t="s">
+      <c r="C102" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="D102" s="59">
+      <c r="D102" s="33">
         <v>4</v>
       </c>
-      <c r="E102" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="F102" s="62">
+      <c r="E102" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F102" s="36">
         <v>4</v>
       </c>
-      <c r="G102" s="61">
+      <c r="G102" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="57">
+      <c r="A103" s="31">
         <v>45819</v>
       </c>
-      <c r="B103" s="58" t="s">
+      <c r="B103" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C103" s="59" t="s">
+      <c r="C103" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="D103" s="59">
+      <c r="D103" s="33">
         <v>4</v>
       </c>
-      <c r="E103" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="F103" s="64">
+      <c r="E103" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F103" s="38">
         <v>4</v>
       </c>
-      <c r="G103" s="61">
+      <c r="G103" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A104" s="47">
+      <c r="A104" s="45">
         <v>45820</v>
       </c>
-      <c r="B104" s="48" t="s">
+      <c r="B104" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C104" s="39" t="s">
+      <c r="C104" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D104" s="39">
-        <v>2</v>
-      </c>
-      <c r="E104" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F104" s="44">
+      <c r="D104" s="24">
+        <v>2</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F104" s="57">
         <v>4</v>
       </c>
-      <c r="G104" s="45">
+      <c r="G104" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="38"/>
-      <c r="B105" s="35"/>
-      <c r="C105" s="22" t="s">
+      <c r="A105" s="47"/>
+      <c r="B105" s="41"/>
+      <c r="C105" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D105" s="22">
-        <v>2</v>
-      </c>
-      <c r="E105" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F105" s="26"/>
-      <c r="G105" s="31">
+      <c r="D105" s="18">
+        <v>2</v>
+      </c>
+      <c r="E105" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F105" s="58"/>
+      <c r="G105" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A106" s="47">
+      <c r="A106" s="45">
         <v>45821</v>
       </c>
-      <c r="B106" s="48" t="s">
+      <c r="B106" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C106" s="39" t="s">
+      <c r="C106" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="D106" s="39">
-        <v>2</v>
-      </c>
-      <c r="E106" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F106" s="49">
+      <c r="D106" s="24">
+        <v>2</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F106" s="42">
         <v>4</v>
       </c>
-      <c r="G106" s="45">
+      <c r="G106" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="38"/>
-      <c r="B107" s="35"/>
-      <c r="C107" s="22" t="s">
+      <c r="A107" s="47"/>
+      <c r="B107" s="41"/>
+      <c r="C107" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D107" s="22">
-        <v>2</v>
-      </c>
-      <c r="E107" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F107" s="29"/>
-      <c r="G107" s="31">
+      <c r="D107" s="18">
+        <v>2</v>
+      </c>
+      <c r="E107" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F107" s="44"/>
+      <c r="G107" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A108" s="47">
+      <c r="A108" s="45">
         <v>45824</v>
       </c>
-      <c r="B108" s="48" t="s">
+      <c r="B108" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="39" t="s">
+      <c r="C108" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="D108" s="39">
-        <v>2</v>
-      </c>
-      <c r="E108" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F108" s="49">
+      <c r="D108" s="24">
+        <v>2</v>
+      </c>
+      <c r="E108" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F108" s="42">
         <v>4</v>
       </c>
-      <c r="G108" s="45">
+      <c r="G108" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="38"/>
-      <c r="B109" s="35"/>
-      <c r="C109" s="22" t="s">
+      <c r="A109" s="47"/>
+      <c r="B109" s="41"/>
+      <c r="C109" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D109" s="22">
-        <v>2</v>
-      </c>
-      <c r="E109" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F109" s="29"/>
-      <c r="G109" s="31">
+      <c r="D109" s="18">
+        <v>2</v>
+      </c>
+      <c r="E109" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F109" s="44"/>
+      <c r="G109" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A110" s="47">
+      <c r="A110" s="45">
         <v>45825</v>
       </c>
-      <c r="B110" s="48" t="s">
+      <c r="B110" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C110" s="39" t="s">
+      <c r="C110" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="D110" s="39">
-        <v>2</v>
-      </c>
-      <c r="E110" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F110" s="49">
+      <c r="D110" s="24">
+        <v>2</v>
+      </c>
+      <c r="E110" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F110" s="42">
         <v>4</v>
       </c>
-      <c r="G110" s="45">
+      <c r="G110" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="38"/>
-      <c r="B111" s="35"/>
-      <c r="C111" s="22" t="s">
+      <c r="A111" s="47"/>
+      <c r="B111" s="41"/>
+      <c r="C111" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D111" s="22">
-        <v>2</v>
-      </c>
-      <c r="E111" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F111" s="29"/>
-      <c r="G111" s="31">
+      <c r="D111" s="18">
+        <v>2</v>
+      </c>
+      <c r="E111" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F111" s="44"/>
+      <c r="G111" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A112" s="47">
+      <c r="A112" s="45">
         <v>45826</v>
       </c>
-      <c r="B112" s="48" t="s">
+      <c r="B112" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C112" s="39" t="s">
+      <c r="C112" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="D112" s="39">
-        <v>2</v>
-      </c>
-      <c r="E112" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F112" s="49">
+      <c r="D112" s="24">
+        <v>2</v>
+      </c>
+      <c r="E112" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F112" s="42">
         <v>4</v>
       </c>
-      <c r="G112" s="45">
+      <c r="G112" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="38"/>
-      <c r="B113" s="35"/>
-      <c r="C113" s="22" t="s">
+      <c r="A113" s="47"/>
+      <c r="B113" s="41"/>
+      <c r="C113" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D113" s="22">
-        <v>2</v>
-      </c>
-      <c r="E113" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F113" s="29"/>
-      <c r="G113" s="31">
+      <c r="D113" s="18">
+        <v>2</v>
+      </c>
+      <c r="E113" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F113" s="44"/>
+      <c r="G113" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A114" s="47">
+      <c r="A114" s="45">
         <v>45827</v>
       </c>
-      <c r="B114" s="48" t="s">
+      <c r="B114" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C114" s="39" t="s">
+      <c r="C114" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="D114" s="39">
-        <v>2</v>
-      </c>
-      <c r="E114" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F114" s="49">
+      <c r="D114" s="24">
+        <v>2</v>
+      </c>
+      <c r="E114" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F114" s="42">
         <v>4</v>
       </c>
-      <c r="G114" s="45">
+      <c r="G114" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="38"/>
-      <c r="B115" s="35"/>
-      <c r="C115" s="22" t="s">
+      <c r="A115" s="47"/>
+      <c r="B115" s="41"/>
+      <c r="C115" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D115" s="22">
-        <v>2</v>
-      </c>
-      <c r="E115" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F115" s="29"/>
-      <c r="G115" s="31">
+      <c r="D115" s="18">
+        <v>2</v>
+      </c>
+      <c r="E115" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F115" s="44"/>
+      <c r="G115" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A116" s="47">
+      <c r="A116" s="45">
         <v>45828</v>
       </c>
-      <c r="B116" s="48" t="s">
+      <c r="B116" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C116" s="39" t="s">
+      <c r="C116" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="D116" s="39">
-        <v>2</v>
-      </c>
-      <c r="E116" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F116" s="49">
+      <c r="D116" s="24">
+        <v>2</v>
+      </c>
+      <c r="E116" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F116" s="42">
         <v>4</v>
       </c>
-      <c r="G116" s="45">
+      <c r="G116" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="38"/>
-      <c r="B117" s="35"/>
-      <c r="C117" s="22" t="s">
+      <c r="A117" s="47"/>
+      <c r="B117" s="41"/>
+      <c r="C117" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D117" s="22">
-        <v>2</v>
-      </c>
-      <c r="E117" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F117" s="29"/>
-      <c r="G117" s="31">
+      <c r="D117" s="18">
+        <v>2</v>
+      </c>
+      <c r="E117" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F117" s="44"/>
+      <c r="G117" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A118" s="47">
+      <c r="A118" s="45">
         <v>45831</v>
       </c>
-      <c r="B118" s="48" t="s">
+      <c r="B118" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C118" s="39" t="s">
+      <c r="C118" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="D118" s="39">
-        <v>2</v>
-      </c>
-      <c r="E118" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F118" s="49">
+      <c r="D118" s="24">
+        <v>2</v>
+      </c>
+      <c r="E118" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F118" s="42">
         <v>4</v>
       </c>
-      <c r="G118" s="45">
+      <c r="G118" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="38"/>
-      <c r="B119" s="35"/>
-      <c r="C119" s="22" t="s">
+      <c r="A119" s="47"/>
+      <c r="B119" s="41"/>
+      <c r="C119" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D119" s="22">
-        <v>2</v>
-      </c>
-      <c r="E119" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F119" s="29"/>
-      <c r="G119" s="31">
+      <c r="D119" s="18">
+        <v>2</v>
+      </c>
+      <c r="E119" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F119" s="44"/>
+      <c r="G119" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A120" s="47">
+      <c r="A120" s="45">
         <v>45801</v>
       </c>
-      <c r="B120" s="48" t="s">
+      <c r="B120" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C120" s="39" t="s">
+      <c r="C120" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="D120" s="39">
-        <v>2</v>
-      </c>
-      <c r="E120" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F120" s="49">
+      <c r="D120" s="24">
+        <v>2</v>
+      </c>
+      <c r="E120" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F120" s="42">
         <v>4</v>
       </c>
-      <c r="G120" s="45">
+      <c r="G120" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="38"/>
-      <c r="B121" s="35"/>
-      <c r="C121" s="22" t="s">
+      <c r="A121" s="47"/>
+      <c r="B121" s="41"/>
+      <c r="C121" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D121" s="22">
-        <v>2</v>
-      </c>
-      <c r="E121" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F121" s="29"/>
-      <c r="G121" s="31">
+      <c r="D121" s="18">
+        <v>2</v>
+      </c>
+      <c r="E121" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F121" s="44"/>
+      <c r="G121" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A122" s="50"/>
-      <c r="B122" s="32"/>
-      <c r="C122" s="15"/>
-      <c r="D122" s="15"/>
-      <c r="E122" s="15"/>
-      <c r="F122" s="51"/>
-      <c r="G122" s="24"/>
+      <c r="A122" s="28"/>
+      <c r="B122" s="23"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="20"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A123" s="50"/>
-      <c r="B123" s="32"/>
-      <c r="C123" s="15"/>
-      <c r="D123" s="15"/>
-      <c r="E123" s="15"/>
-      <c r="F123" s="51"/>
-      <c r="G123" s="24"/>
+      <c r="A123" s="28"/>
+      <c r="B123" s="23"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="20"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A124" s="50"/>
-      <c r="B124" s="32"/>
-      <c r="C124" s="15"/>
-      <c r="D124" s="15"/>
-      <c r="E124" s="15"/>
-      <c r="F124" s="17"/>
-      <c r="G124" s="24"/>
+      <c r="A124" s="28"/>
+      <c r="B124" s="23"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A125" s="50"/>
-      <c r="B125" s="32"/>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="15"/>
-      <c r="F125" s="17"/>
-      <c r="G125" s="24"/>
+      <c r="A125" s="28"/>
+      <c r="B125" s="23"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A126" s="50"/>
-      <c r="B126" s="32"/>
-      <c r="C126" s="15"/>
-      <c r="D126" s="15"/>
-      <c r="E126" s="15"/>
-      <c r="F126" s="17"/>
-      <c r="G126" s="24"/>
+      <c r="A126" s="28"/>
+      <c r="B126" s="23"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
     </row>
     <row r="127" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B127" s="56"/>
+      <c r="B127" s="23"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -3517,7 +3496,10 @@
     <row r="129" spans="2:6" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.5">
       <c r="B129" s="11"/>
       <c r="D129" s="8"/>
-      <c r="E129"/>
+      <c r="E129">
+        <f>SUM(F9:F121)</f>
+        <v>200</v>
+      </c>
       <c r="F129" s="6"/>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.5">

</xml_diff>